<commit_message>
Ver-3.0.1 Methods for centrality metrics of multi-graphs have been revised.
</commit_message>
<xml_diff>
--- a/result/All_centrality.xlsx
+++ b/result/All_centrality.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,32 +441,92 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>('Betweenness', 'node')</t>
+          <t>('Betweenness', 'node1')</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>('Betweenness', 'value')</t>
+          <t>('Betweenness', 'value1')</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>('Closeness', 'node')</t>
+          <t>('Betweenness', 'node2')</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>('Closeness', 'value')</t>
+          <t>('Betweenness', 'value2')</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>('Degree', 'node')</t>
+          <t>('Betweenness', 'node3')</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>('Degree', 'value')</t>
+          <t>('Betweenness', 'value3')</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>('Closeness', 'node1')</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>('Closeness', 'value1')</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>('Closeness', 'node2')</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>('Closeness', 'value2')</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>('Closeness', 'node3')</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>('Closeness', 'value3')</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>('Degree', 'node1')</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>('Degree', 'value1')</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>('Degree', 'node2')</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>('Degree', 'value2')</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>('Degree', 'node3')</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>('Degree', 'value3')</t>
         </is>
       </c>
     </row>
@@ -486,19 +546,67 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>케플러법칙</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.1478279317385609</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>행성</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="G2" t="n">
+        <v>0.1410976472855235</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>행성</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
         <v>0.3500268749776042</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>태양계</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>0.2779661016949153</v>
+      <c r="K2" t="n">
+        <v>0.3492884216548666</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>케플러법칙</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>0.3083104503992677</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>태양계</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>82</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>행성</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>80</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>케플러법칙</t>
+        </is>
+      </c>
+      <c r="S2" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="3">
@@ -513,7 +621,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.2376785219437501</v>
+        <v>0.2296290410994625</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -521,15 +629,63 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.3496697131481313</v>
+        <v>0.202396998207084</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>표본추출</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0.1656861221582649</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>비확률적표본추출</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0.3466749191940032</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>확률적표본추출</t>
         </is>
       </c>
-      <c r="G3" t="n">
-        <v>0.4465116279069767</v>
+      <c r="K3" t="n">
+        <v>0.3453567636077142</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>표본추출</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>0.3186976450134345</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>확률적표본추출</t>
+        </is>
+      </c>
+      <c r="O3" t="n">
+        <v>98</v>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>비확률적표본추출</t>
+        </is>
+      </c>
+      <c r="Q3" t="n">
+        <v>88</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>표본추출</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>82</v>
       </c>
     </row>
     <row r="4">
@@ -544,23 +700,71 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.230513899143882</v>
+        <v>0.2291077994660412</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>데이터베이스</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.2008070968266106</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>non-RDBMS</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>0.1603612529923504</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>RDBMS</t>
         </is>
       </c>
-      <c r="E4" t="n">
-        <v>0.3678262388847509</v>
-      </c>
-      <c r="F4" t="inlineStr">
+      <c r="I4" t="n">
+        <v>0.3687791566020688</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>데이터베이스</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>0.3585610943284599</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>non-RDBMS</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>0.3480409644215124</v>
+      </c>
+      <c r="N4" t="inlineStr">
         <is>
           <t>RDBMS</t>
         </is>
       </c>
-      <c r="G4" t="n">
-        <v>0.5017793594306049</v>
+      <c r="O4" t="n">
+        <v>141</v>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>데이터베이스</t>
+        </is>
+      </c>
+      <c r="Q4" t="n">
+        <v>133</v>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>non-RDBMS</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ver-3.0.2 Centrality metrics of multi-graphs have been changed to `unweighted`.
</commit_message>
<xml_diff>
--- a/result/All_centrality.xlsx
+++ b/result/All_centrality.xlsx
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="O2" t="n">
-        <v>82</v>
+        <v>0.2779661016949153</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>80</v>
+        <v>0.2711864406779661</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="S2" t="n">
-        <v>70</v>
+        <v>0.2372881355932203</v>
       </c>
     </row>
     <row r="3">
@@ -669,7 +669,7 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>98</v>
+        <v>0.4414414414414414</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
@@ -677,7 +677,7 @@
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>88</v>
+        <v>0.3963963963963964</v>
       </c>
       <c r="R3" t="inlineStr">
         <is>
@@ -685,7 +685,7 @@
         </is>
       </c>
       <c r="S3" t="n">
-        <v>82</v>
+        <v>0.3693693693693694</v>
       </c>
     </row>
     <row r="4">
@@ -748,7 +748,7 @@
         </is>
       </c>
       <c r="O4" t="n">
-        <v>141</v>
+        <v>0.5017793594306049</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
@@ -756,7 +756,7 @@
         </is>
       </c>
       <c r="Q4" t="n">
-        <v>133</v>
+        <v>0.4733096085409252</v>
       </c>
       <c r="R4" t="inlineStr">
         <is>
@@ -764,7 +764,7 @@
         </is>
       </c>
       <c r="S4" t="n">
-        <v>120</v>
+        <v>0.4270462633451957</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ver-3.1.0 1. Methods for consensus metrics have been added. 2. Result data have been added.
</commit_message>
<xml_diff>
--- a/result/All_centrality.xlsx
+++ b/result/All_centrality.xlsx
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.1983368870485608</v>
+        <v>0.1741947494915157</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.1478279317385609</v>
+        <v>0.09111564259528658</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -558,39 +558,39 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0.1410976472855235</v>
+        <v>0.07877662572384592</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>태양계</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0.2371271638948406</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>행성</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>0.3500268749776042</v>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="n">
+        <v>0.2188866128260067</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>위성</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>0.2096034752284752</v>
+      </c>
+      <c r="N2" t="inlineStr">
         <is>
           <t>태양계</t>
         </is>
       </c>
-      <c r="K2" t="n">
-        <v>0.3492884216548666</v>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>케플러법칙</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
-        <v>0.3083104503992677</v>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>태양계</t>
-        </is>
-      </c>
       <c r="O2" t="n">
-        <v>0.2779661016949153</v>
+        <v>0.2053872053872054</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
@@ -598,15 +598,15 @@
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>0.2711864406779661</v>
+        <v>0.1750841750841751</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>케플러법칙</t>
+          <t>목성</t>
         </is>
       </c>
       <c r="S2" t="n">
-        <v>0.2372881355932203</v>
+        <v>0.1414141414141414</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Ver-3.1.1 1. The subgraph coverage metric has been changed. 2. Mean values of centrality metrics have been added. 3. Minor bugs at data loading have been fixed.
</commit_message>
<xml_diff>
--- a/result/All_centrality.xlsx
+++ b/result/All_centrality.xlsx
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.1741947494915157</v>
+        <v>0.1983368870485608</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.09111564259528658</v>
+        <v>0.1478279317385609</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -558,55 +558,55 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0.07877662572384592</v>
+        <v>0.1410976472855235</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>행성</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0.3500268749776042</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>태양계</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>0.2371271638948406</v>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="n">
+        <v>0.3492884216548666</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>케플러법칙</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>0.3083104503992677</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>태양계</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>0.2779661016949153</v>
+      </c>
+      <c r="P2" t="inlineStr">
         <is>
           <t>행성</t>
         </is>
       </c>
-      <c r="K2" t="n">
-        <v>0.2188866128260067</v>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>위성</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
-        <v>0.2096034752284752</v>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>태양계</t>
-        </is>
-      </c>
-      <c r="O2" t="n">
-        <v>0.2053872053872054</v>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>행성</t>
-        </is>
-      </c>
       <c r="Q2" t="n">
-        <v>0.1750841750841751</v>
+        <v>0.2711864406779661</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>목성</t>
+          <t>케플러법칙</t>
         </is>
       </c>
       <c r="S2" t="n">
-        <v>0.1414141414141414</v>
+        <v>0.2372881355932203</v>
       </c>
     </row>
     <row r="3">

</xml_diff>